<commit_message>
mona minta yang lulus jadi layak
</commit_message>
<xml_diff>
--- a/DATA TESTING & DATA UJI/datatesting_mona.xlsx
+++ b/DATA TESTING & DATA UJI/datatesting_mona.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kickymaulana\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kickymaulana\Downloads\mona\knn_algorithm\DATA TESTING &amp; DATA UJI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3736DDB2-EB62-4450-B865-9B3479C3F076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1CD9E4-ACBA-4B55-A078-D3A55DC25036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B37114CE-FFD3-4359-84AD-C162DBE58A15}"/>
   </bookViews>
@@ -883,7 +883,7 @@
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+      <selection activeCell="G2" sqref="G2:G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -983,7 +983,7 @@
         <v>73</v>
       </c>
       <c r="G4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1466,7 +1466,7 @@
         <v>147</v>
       </c>
       <c r="G25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1558,7 +1558,7 @@
         <v>132</v>
       </c>
       <c r="G29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1673,7 +1673,7 @@
         <v>88</v>
       </c>
       <c r="G34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1742,7 +1742,7 @@
         <v>73</v>
       </c>
       <c r="G37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1972,7 +1972,7 @@
         <v>41</v>
       </c>
       <c r="G47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -1995,7 +1995,7 @@
         <v>29</v>
       </c>
       <c r="G48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2018,7 +2018,7 @@
         <v>29</v>
       </c>
       <c r="G49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -2041,7 +2041,7 @@
         <v>29</v>
       </c>
       <c r="G50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -2064,7 +2064,7 @@
         <v>32</v>
       </c>
       <c r="G51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -2087,7 +2087,7 @@
         <v>35</v>
       </c>
       <c r="G52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -2110,7 +2110,7 @@
         <v>59</v>
       </c>
       <c r="G53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -2156,7 +2156,7 @@
         <v>44</v>
       </c>
       <c r="G55" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -2179,7 +2179,7 @@
         <v>37</v>
       </c>
       <c r="G56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -2202,7 +2202,7 @@
         <v>18</v>
       </c>
       <c r="G57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -2225,7 +2225,7 @@
         <v>15</v>
       </c>
       <c r="G58" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -2248,7 +2248,7 @@
         <v>6</v>
       </c>
       <c r="G59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -2271,7 +2271,7 @@
         <v>59</v>
       </c>
       <c r="G60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -2294,7 +2294,7 @@
         <v>18</v>
       </c>
       <c r="G61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -2317,7 +2317,7 @@
         <v>15</v>
       </c>
       <c r="G62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -2340,7 +2340,7 @@
         <v>44</v>
       </c>
       <c r="G63" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -2363,7 +2363,7 @@
         <v>15</v>
       </c>
       <c r="G64" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2386,7 +2386,7 @@
         <v>15</v>
       </c>
       <c r="G65" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2409,7 +2409,7 @@
         <v>15</v>
       </c>
       <c r="G66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -2432,7 +2432,7 @@
         <v>21</v>
       </c>
       <c r="G67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -2478,7 +2478,7 @@
         <v>18</v>
       </c>
       <c r="G69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -2501,7 +2501,7 @@
         <v>18</v>
       </c>
       <c r="G70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -2524,7 +2524,7 @@
         <v>35</v>
       </c>
       <c r="G71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -2547,7 +2547,7 @@
         <v>24</v>
       </c>
       <c r="G72" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -2593,7 +2593,7 @@
         <v>44</v>
       </c>
       <c r="G74" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -2616,7 +2616,7 @@
         <v>66</v>
       </c>
       <c r="G75" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -2639,7 +2639,7 @@
         <v>29</v>
       </c>
       <c r="G76" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -2662,7 +2662,7 @@
         <v>65</v>
       </c>
       <c r="G77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -2685,7 +2685,7 @@
         <v>29</v>
       </c>
       <c r="G78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -2731,7 +2731,7 @@
         <v>29</v>
       </c>
       <c r="G80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -2754,7 +2754,7 @@
         <v>37</v>
       </c>
       <c r="G81" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>